<commit_message>
fix typo in column description
</commit_message>
<xml_diff>
--- a/public/ExcelTemplates/PurchasesReportNew.xlsx
+++ b/public/ExcelTemplates/PurchasesReportNew.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmoud.fayez\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmoud.fayez\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312905C5-FEDE-47C0-9168-8255DB60BEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7799E9B0-21DF-45FF-8869-9789BCC517B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,9 +115,6 @@
     <t>ضريبة القيمة المضافة</t>
   </si>
   <si>
-    <t>اجمالى المبيعات قبل الضريبة</t>
-  </si>
-  <si>
     <t>القيمة</t>
   </si>
   <si>
@@ -125,6 +122,9 @@
   </si>
   <si>
     <t>رقم التسجيل الضريبي</t>
+  </si>
+  <si>
+    <t>اجمالى المشتريات قبل الضريبة</t>
   </si>
 </sst>
 </file>
@@ -832,7 +832,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -968,10 +968,10 @@
         <v>3</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="19" t="s">
         <v>6</v>
@@ -983,7 +983,7 @@
         <v>8</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>5</v>
@@ -992,7 +992,7 @@
         <v>4</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>5</v>
@@ -1001,7 +1001,7 @@
         <v>4</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>5</v>
@@ -1010,7 +1010,7 @@
         <v>4</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>5</v>
@@ -1019,7 +1019,7 @@
         <v>4</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="W3" s="5" t="s">
         <v>5</v>
@@ -1028,7 +1028,7 @@
         <v>4</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Z3" s="5" t="s">
         <v>5</v>
@@ -1037,7 +1037,7 @@
         <v>4</v>
       </c>
       <c r="AB3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC3" s="5" t="s">
         <v>5</v>
@@ -1046,7 +1046,7 @@
         <v>4</v>
       </c>
       <c r="AE3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AF3" s="5" t="s">
         <v>5</v>
@@ -1055,7 +1055,7 @@
         <v>4</v>
       </c>
       <c r="AH3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AI3" s="5" t="s">
         <v>5</v>
@@ -1064,7 +1064,7 @@
         <v>4</v>
       </c>
       <c r="AK3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AL3" s="5" t="s">
         <v>5</v>
@@ -1073,7 +1073,7 @@
         <v>4</v>
       </c>
       <c r="AN3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AO3" s="5" t="s">
         <v>5</v>
@@ -1082,7 +1082,7 @@
         <v>4</v>
       </c>
       <c r="AQ3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AR3" s="5" t="s">
         <v>5</v>
@@ -1091,7 +1091,7 @@
         <v>4</v>
       </c>
       <c r="AT3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AU3" s="5" t="s">
         <v>5</v>
@@ -1100,7 +1100,7 @@
         <v>4</v>
       </c>
       <c r="AW3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>